<commit_message>
case study1 & extent reporting
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YOGESH RANA\Desktop\SDET_Automation2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{CB63EA2A-6DC3-4640-AD93-A08864CFFACE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C1EE5E-2F41-4B73-AFFD-8CAE70B6D66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{E99C8F6D-CCD1-4BE2-9253-50201E74F457}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{E99C8F6D-CCD1-4BE2-9253-50201E74F457}"/>
   </bookViews>
   <sheets>
-    <sheet name="Info" r:id="rId1" sheetId="1"/>
-    <sheet name="Test1" r:id="rId2" sheetId="2"/>
+    <sheet name="Info" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData1" sheetId="2" r:id="rId2"/>
+    <sheet name="TestOutput1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -149,13 +150,27 @@
   </si>
   <si>
     <t>E0008</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>info@orangehrm.com</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>OrangeHRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -187,18 +202,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -215,10 +246,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -253,7 +284,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -305,7 +336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -416,21 +447,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -447,7 +478,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -499,15 +530,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9DFA3C-5DB0-4035-AF03-052D1CFE2192}">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9DFA3C-5DB0-4035-AF03-052D1CFE2192}">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
@@ -720,18 +751,65 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35669928-2AC0-45BE-9E1E-68F4AAC57B93}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35669928-2AC0-45BE-9E1E-68F4AAC57B93}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3783E919-F056-443B-829C-1B6A4EF7EF85}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>